<commit_message>
Updated to reflect recent changes.
</commit_message>
<xml_diff>
--- a/docs/Software Engg/#01 Project Management/Phresco Iteration Plan.xlsx
+++ b/docs/Software Engg/#01 Project Management/Phresco Iteration Plan.xlsx
@@ -48,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="0">
+    <comment ref="C6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="102">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -424,6 +424,24 @@
   </si>
   <si>
     <t>Service Gateway. Necessary for mobile?</t>
+  </si>
+  <si>
+    <t>Code Quality Guidelines and Checklists</t>
+  </si>
+  <si>
+    <t>Emma, CheckStyle, PHPLint et al.</t>
+  </si>
+  <si>
+    <t>Web (Enterprise Java)</t>
+  </si>
+  <si>
+    <t>Web (Sharepoint)</t>
+  </si>
+  <si>
+    <t>Tomcat/Spring/Struts/Hibernate</t>
+  </si>
+  <si>
+    <t>WebPart development, MasterPage Development</t>
   </si>
 </sst>
 </file>
@@ -525,7 +543,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -577,6 +595,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -622,8 +646,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H45" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A1:H45"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H48" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A1:H48"/>
   <tableColumns count="8">
     <tableColumn id="1" name="Sl. No." dataDxfId="6">
       <calculatedColumnFormula>A1+0.1</calculatedColumnFormula>
@@ -939,10 +963,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H45"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,7 +1043,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="26">
         <f>A3+0.1</f>
         <v>1.3000000000000003</v>
       </c>
@@ -1027,102 +1051,102 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>59</v>
+        <v>100</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="26">
         <f>A4+0.1</f>
         <v>1.4000000000000004</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="23" t="s">
+      <c r="C5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>2.1</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>8</v>
+        <f>A5+0.1</f>
+        <v>1.5000000000000004</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="8">
         <f>A6+0.1</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="19" t="s">
+        <v>1.6000000000000005</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="23" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <f>A7+0.1</f>
-        <v>2.3000000000000003</v>
+        <v>2.1</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f>A8+0.1</f>
-        <v>2.4000000000000004</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>46</v>
       </c>
       <c r="E9" s="24" t="s">
         <v>86</v>
@@ -1131,126 +1155,126 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f>A9+0.1</f>
-        <v>2.5000000000000004</v>
+        <v>2.3000000000000003</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>46</v>
+        <v>50</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="E10" s="24" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <f>A10+0.1</f>
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <f>A11+0.1</f>
+        <v>2.5000000000000004</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="26">
+        <f>A12+0.1</f>
         <v>2.6000000000000005</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B13" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C13" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="8">
+        <f>A13+0.1</f>
+        <v>2.7000000000000006</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D14" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E14" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>3.1</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <f t="shared" ref="A13:A19" si="0">A12+0.1</f>
-        <v>3.2</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <f t="shared" si="0"/>
-        <v>3.3000000000000003</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="E14" s="24" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <f t="shared" si="0"/>
-        <v>3.4000000000000004</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <f t="shared" si="0"/>
-        <v>3.5000000000000004</v>
+        <f t="shared" ref="A16:A22" si="0">A15+0.1</f>
+        <v>3.2</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>60</v>
+        <v>11</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>46</v>
       </c>
       <c r="E16" s="24" t="s">
         <v>87</v>
@@ -1259,16 +1283,16 @@
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
-        <v>3.6000000000000005</v>
+        <v>3.3000000000000003</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>56</v>
+        <v>12</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>46</v>
       </c>
       <c r="E17" s="24" t="s">
         <v>87</v>
@@ -1277,16 +1301,16 @@
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
-        <v>3.7000000000000006</v>
+        <v>3.4000000000000004</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="E18" s="24" t="s">
         <v>87</v>
@@ -1295,16 +1319,16 @@
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
-        <v>3.8000000000000007</v>
+        <v>3.5000000000000004</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>46</v>
+        <v>14</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="E19" s="24" t="s">
         <v>87</v>
@@ -1312,125 +1336,125 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <f>A19+0.1</f>
-        <v>3.9000000000000008</v>
+        <f t="shared" si="0"/>
+        <v>3.6000000000000005</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>46</v>
+        <v>15</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="E20" s="24" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="21" t="s">
-        <v>79</v>
+      <c r="A21" s="1">
+        <f t="shared" si="0"/>
+        <v>3.7000000000000006</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>46</v>
+        <v>16</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>45</v>
       </c>
       <c r="E21" s="24" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="14" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <f t="shared" si="0"/>
+        <v>3.8000000000000007</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <f>A22+0.1</f>
+        <v>3.9000000000000008</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B25" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C25" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D25" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E25" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
         <v>4.0999999999999996</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <f>A23+0.1</f>
-        <v>4.1999999999999993</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <f t="shared" ref="A25:A31" si="1">A24+0.1</f>
-        <v>4.2999999999999989</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <f t="shared" si="1"/>
-        <v>4.3999999999999986</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>88</v>
@@ -1438,17 +1462,17 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <f t="shared" si="1"/>
-        <v>4.4999999999999982</v>
+        <f>A26+0.1</f>
+        <v>4.1999999999999993</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="19" t="s">
-        <v>46</v>
+        <v>77</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>88</v>
@@ -1456,17 +1480,17 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <f t="shared" si="1"/>
-        <v>4.5999999999999979</v>
+        <f t="shared" ref="A28:A34" si="1">A27+0.1</f>
+        <v>4.2999999999999989</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>46</v>
+        <v>20</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>88</v>
@@ -1475,16 +1499,16 @@
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f t="shared" si="1"/>
-        <v>4.6999999999999975</v>
+        <v>4.3999999999999986</v>
       </c>
       <c r="B29" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>46</v>
+        <v>21</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>88</v>
@@ -1493,16 +1517,16 @@
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f t="shared" si="1"/>
-        <v>4.7999999999999972</v>
+        <v>4.4999999999999982</v>
       </c>
       <c r="B30" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>62</v>
+        <v>22</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>46</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>88</v>
@@ -1511,141 +1535,141 @@
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" si="1"/>
-        <v>4.8999999999999968</v>
+        <v>4.5999999999999979</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>65</v>
+        <v>23</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>46</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="21" t="s">
-        <v>43</v>
+      <c r="A32" s="1">
+        <f t="shared" si="1"/>
+        <v>4.6999999999999975</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>66</v>
+        <v>24</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>46</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="21" t="s">
-        <v>63</v>
+      <c r="A33" s="1">
+        <f t="shared" si="1"/>
+        <v>4.7999999999999972</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>18</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="14" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <f t="shared" si="1"/>
+        <v>4.8999999999999968</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B37" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C37" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D37" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E37" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-    </row>
-    <row r="35" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
         <v>5.0999999999999996</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
-        <f t="shared" ref="A36:A43" si="2">A35+0.1</f>
-        <v>5.1999999999999993</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
-        <f>A36+0.1</f>
-        <v>5.2999999999999989</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
-        <f>A37+0.1</f>
-        <v>5.3999999999999986</v>
       </c>
       <c r="B38" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D38" s="19" t="s">
-        <v>46</v>
+        <v>30</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>89</v>
@@ -1653,17 +1677,17 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <f t="shared" si="2"/>
-        <v>5.4999999999999982</v>
+        <f t="shared" ref="A39:A46" si="2">A38+0.1</f>
+        <v>5.1999999999999993</v>
       </c>
       <c r="B39" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>89</v>
@@ -1671,17 +1695,17 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <f t="shared" si="2"/>
-        <v>5.5999999999999979</v>
+        <f>A39+0.1</f>
+        <v>5.2999999999999989</v>
       </c>
       <c r="B40" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>46</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>89</v>
@@ -1689,17 +1713,17 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <f t="shared" si="2"/>
-        <v>5.6999999999999975</v>
+        <f>A40+0.1</f>
+        <v>5.3999999999999986</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>73</v>
+        <v>32</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>46</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>89</v>
@@ -1708,16 +1732,16 @@
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <f t="shared" si="2"/>
-        <v>5.7999999999999972</v>
+        <v>5.4999999999999982</v>
       </c>
       <c r="B42" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>89</v>
@@ -1726,57 +1750,111 @@
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <f t="shared" si="2"/>
-        <v>5.8999999999999968</v>
+        <v>5.5999999999999979</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D43" s="19" t="s">
-        <v>46</v>
+        <v>34</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="21" t="s">
-        <v>70</v>
+      <c r="A44" s="1">
+        <f t="shared" si="2"/>
+        <v>5.6999999999999975</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D44" s="19" t="s">
-        <v>46</v>
+        <v>35</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="16" t="s">
-        <v>71</v>
+      <c r="A45" s="1">
+        <f t="shared" si="2"/>
+        <v>5.7999999999999972</v>
       </c>
       <c r="B45" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C45" s="17" t="s">
+      <c r="C45" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <f t="shared" si="2"/>
+        <v>5.8999999999999968</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D45" s="17" t="s">
+      <c r="D48" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="E45" s="22" t="s">
+      <c r="E48" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
-      <c r="H45" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>